<commit_message>
docs: add responsibility matrix
</commit_message>
<xml_diff>
--- a/docs/resources/tables/cost-analysis-2023-02-03.xlsx
+++ b/docs/resources/tables/cost-analysis-2023-02-03.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jahrim\Desktop\Projects\pm-project\docs\resources\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E2D696-DBE9-46AE-B877-3F99C8151ACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E774235-D9B2-4B8C-80D8-0219AF4A4D66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1187,7 +1187,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1281,6 +1281,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="5" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1592,8 +1595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A138" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J168" sqref="J168"/>
+    <sheetView tabSelected="1" topLeftCell="A147" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C177" sqref="C177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1609,10 +1612,10 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="38" t="s">
         <v>275</v>
       </c>
-      <c r="B2" s="38"/>
+      <c r="B2" s="39"/>
       <c r="C2" s="30">
         <v>19.2</v>
       </c>
@@ -3786,11 +3789,11 @@
         <v>105</v>
       </c>
       <c r="C72" s="6">
-        <v>21.5</v>
+        <v>10.75</v>
       </c>
       <c r="D72" s="10">
         <f>C72*1.25*1.33</f>
-        <v>35.743749999999999</v>
+        <v>17.871874999999999</v>
       </c>
       <c r="E72" s="11" t="s">
         <v>272</v>
@@ -3800,18 +3803,18 @@
       </c>
       <c r="G72" s="28">
         <f t="shared" ref="G72:G74" si="45">F72*D72</f>
-        <v>661.25937499999998</v>
+        <v>330.62968749999999</v>
       </c>
       <c r="H72" s="28">
         <v>2200</v>
       </c>
       <c r="I72" s="28">
         <f t="shared" ref="I72:I74" si="46">PRODUCT(D72,$C$2)</f>
-        <v>686.28</v>
+        <v>343.14</v>
       </c>
       <c r="J72" s="28">
         <f t="shared" ref="J72:J74" si="47">SUM(G72:I72)</f>
-        <v>3547.5393750000003</v>
+        <v>2873.7696874999997</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
@@ -3822,11 +3825,11 @@
         <v>107</v>
       </c>
       <c r="C73" s="6">
-        <v>18.5</v>
+        <v>9.25</v>
       </c>
       <c r="D73" s="10">
         <f>C73*1.25*1.33</f>
-        <v>30.756250000000001</v>
+        <v>15.378125000000001</v>
       </c>
       <c r="E73" s="11" t="s">
         <v>272</v>
@@ -3836,18 +3839,18 @@
       </c>
       <c r="G73" s="28">
         <f t="shared" si="45"/>
-        <v>568.99062500000002</v>
+        <v>284.49531250000001</v>
       </c>
       <c r="H73" s="28">
         <v>0</v>
       </c>
       <c r="I73" s="28">
         <f t="shared" si="46"/>
-        <v>590.52</v>
+        <v>295.26</v>
       </c>
       <c r="J73" s="28">
         <f t="shared" si="47"/>
-        <v>1159.5106249999999</v>
+        <v>579.75531249999995</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
@@ -3858,11 +3861,11 @@
         <v>109</v>
       </c>
       <c r="C74" s="6">
-        <v>20.5</v>
+        <v>10.25</v>
       </c>
       <c r="D74" s="10">
         <f>C74*1.25*1.33</f>
-        <v>34.081250000000004</v>
+        <v>17.040625000000002</v>
       </c>
       <c r="E74" s="11" t="s">
         <v>272</v>
@@ -3872,18 +3875,18 @@
       </c>
       <c r="G74" s="28">
         <f t="shared" si="45"/>
-        <v>630.50312500000007</v>
+        <v>315.25156250000003</v>
       </c>
       <c r="H74" s="28">
         <v>0</v>
       </c>
       <c r="I74" s="28">
         <f t="shared" si="46"/>
-        <v>654.36</v>
+        <v>327.18</v>
       </c>
       <c r="J74" s="28">
         <f t="shared" si="47"/>
-        <v>1284.8631250000001</v>
+        <v>642.43156250000004</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
@@ -3910,11 +3913,11 @@
         <v>111</v>
       </c>
       <c r="C76" s="6">
-        <v>21.5</v>
+        <v>10.75</v>
       </c>
       <c r="D76" s="10">
         <f>C76*1.25*1.33</f>
-        <v>35.743749999999999</v>
+        <v>17.871874999999999</v>
       </c>
       <c r="E76" s="11" t="s">
         <v>272</v>
@@ -3924,18 +3927,18 @@
       </c>
       <c r="G76" s="28">
         <f t="shared" ref="G76:G78" si="48">F76*D76</f>
-        <v>661.25937499999998</v>
+        <v>330.62968749999999</v>
       </c>
       <c r="H76" s="28">
         <v>2200</v>
       </c>
       <c r="I76" s="28">
         <f t="shared" ref="I76:I78" si="49">PRODUCT(D76,$C$2)</f>
-        <v>686.28</v>
+        <v>343.14</v>
       </c>
       <c r="J76" s="28">
         <f t="shared" ref="J76:J78" si="50">SUM(G76:I76)</f>
-        <v>3547.5393750000003</v>
+        <v>2873.7696874999997</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
@@ -3946,11 +3949,11 @@
         <v>113</v>
       </c>
       <c r="C77" s="6">
-        <v>20.5</v>
+        <v>10.25</v>
       </c>
       <c r="D77" s="10">
         <f>C77*1.25*1.33</f>
-        <v>34.081250000000004</v>
+        <v>17.040625000000002</v>
       </c>
       <c r="E77" s="11" t="s">
         <v>272</v>
@@ -3960,18 +3963,18 @@
       </c>
       <c r="G77" s="28">
         <f t="shared" si="48"/>
-        <v>630.50312500000007</v>
+        <v>315.25156250000003</v>
       </c>
       <c r="H77" s="28">
         <v>0</v>
       </c>
       <c r="I77" s="28">
         <f t="shared" si="49"/>
-        <v>654.36</v>
+        <v>327.18</v>
       </c>
       <c r="J77" s="28">
         <f t="shared" si="50"/>
-        <v>1284.8631250000001</v>
+        <v>642.43156250000004</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
@@ -3982,11 +3985,11 @@
         <v>115</v>
       </c>
       <c r="C78" s="6">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D78" s="10">
         <f>C78*1.25*1.33</f>
-        <v>36.575000000000003</v>
+        <v>18.287500000000001</v>
       </c>
       <c r="E78" s="11" t="s">
         <v>272</v>
@@ -3996,18 +3999,18 @@
       </c>
       <c r="G78" s="28">
         <f t="shared" si="48"/>
-        <v>676.63750000000005</v>
+        <v>338.31875000000002</v>
       </c>
       <c r="H78" s="28">
         <v>0</v>
       </c>
       <c r="I78" s="28">
         <f t="shared" si="49"/>
-        <v>702.24</v>
+        <v>351.12</v>
       </c>
       <c r="J78" s="28">
         <f t="shared" si="50"/>
-        <v>1378.8775000000001</v>
+        <v>689.43875000000003</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
@@ -4034,11 +4037,11 @@
         <v>117</v>
       </c>
       <c r="C80" s="6">
-        <v>21.5</v>
+        <v>10.75</v>
       </c>
       <c r="D80" s="10">
         <f>C80*1.25*1.33</f>
-        <v>35.743749999999999</v>
+        <v>17.871874999999999</v>
       </c>
       <c r="E80" s="11" t="s">
         <v>272</v>
@@ -4048,18 +4051,18 @@
       </c>
       <c r="G80" s="28">
         <f t="shared" ref="G80:G82" si="51">F80*D80</f>
-        <v>661.25937499999998</v>
+        <v>330.62968749999999</v>
       </c>
       <c r="H80" s="28">
         <v>2200</v>
       </c>
       <c r="I80" s="28">
         <f t="shared" ref="I80:I82" si="52">PRODUCT(D80,$C$2)</f>
-        <v>686.28</v>
+        <v>343.14</v>
       </c>
       <c r="J80" s="28">
         <f t="shared" ref="J80:J82" si="53">SUM(G80:I80)</f>
-        <v>3547.5393750000003</v>
+        <v>2873.7696874999997</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
@@ -4070,11 +4073,11 @@
         <v>119</v>
       </c>
       <c r="C81" s="6">
-        <v>18.5</v>
+        <v>9.25</v>
       </c>
       <c r="D81" s="10">
         <f>C81*1.25*1.33</f>
-        <v>30.756250000000001</v>
+        <v>15.378125000000001</v>
       </c>
       <c r="E81" s="11" t="s">
         <v>272</v>
@@ -4084,18 +4087,18 @@
       </c>
       <c r="G81" s="28">
         <f t="shared" si="51"/>
-        <v>568.99062500000002</v>
+        <v>284.49531250000001</v>
       </c>
       <c r="H81" s="28">
         <v>0</v>
       </c>
       <c r="I81" s="28">
         <f t="shared" si="52"/>
-        <v>590.52</v>
+        <v>295.26</v>
       </c>
       <c r="J81" s="28">
         <f t="shared" si="53"/>
-        <v>1159.5106249999999</v>
+        <v>579.75531249999995</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
@@ -4106,11 +4109,11 @@
         <v>121</v>
       </c>
       <c r="C82" s="6">
-        <v>15.5</v>
+        <v>7.75</v>
       </c>
       <c r="D82" s="10">
         <f>C82*1.25*1.33</f>
-        <v>25.768750000000001</v>
+        <v>12.884375</v>
       </c>
       <c r="E82" s="11" t="s">
         <v>272</v>
@@ -4120,18 +4123,18 @@
       </c>
       <c r="G82" s="28">
         <f t="shared" si="51"/>
-        <v>476.72187500000001</v>
+        <v>238.36093750000001</v>
       </c>
       <c r="H82" s="28">
         <v>0</v>
       </c>
       <c r="I82" s="28">
         <f t="shared" si="52"/>
-        <v>494.76</v>
+        <v>247.38</v>
       </c>
       <c r="J82" s="28">
         <f t="shared" si="53"/>
-        <v>971.48187499999995</v>
+        <v>485.74093749999997</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
@@ -4158,11 +4161,11 @@
         <v>123</v>
       </c>
       <c r="C84" s="6">
-        <v>21.5</v>
+        <v>10.75</v>
       </c>
       <c r="D84" s="10">
         <f>C84*1.25*1.33</f>
-        <v>35.743749999999999</v>
+        <v>17.871874999999999</v>
       </c>
       <c r="E84" s="11" t="s">
         <v>272</v>
@@ -4172,18 +4175,18 @@
       </c>
       <c r="G84" s="28">
         <f t="shared" ref="G84:G86" si="54">F84*D84</f>
-        <v>661.25937499999998</v>
+        <v>330.62968749999999</v>
       </c>
       <c r="H84" s="28">
         <v>2200</v>
       </c>
       <c r="I84" s="28">
         <f t="shared" ref="I84:I86" si="55">PRODUCT(D84,$C$2)</f>
-        <v>686.28</v>
+        <v>343.14</v>
       </c>
       <c r="J84" s="28">
         <f t="shared" ref="J84:J86" si="56">SUM(G84:I84)</f>
-        <v>3547.5393750000003</v>
+        <v>2873.7696874999997</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
@@ -4194,11 +4197,11 @@
         <v>125</v>
       </c>
       <c r="C85" s="6">
-        <v>18.5</v>
+        <v>9.25</v>
       </c>
       <c r="D85" s="10">
         <f>C85*1.25*1.33</f>
-        <v>30.756250000000001</v>
+        <v>15.378125000000001</v>
       </c>
       <c r="E85" s="11" t="s">
         <v>272</v>
@@ -4208,18 +4211,18 @@
       </c>
       <c r="G85" s="28">
         <f t="shared" si="54"/>
-        <v>568.99062500000002</v>
+        <v>284.49531250000001</v>
       </c>
       <c r="H85" s="28">
         <v>0</v>
       </c>
       <c r="I85" s="28">
         <f t="shared" si="55"/>
-        <v>590.52</v>
+        <v>295.26</v>
       </c>
       <c r="J85" s="28">
         <f t="shared" si="56"/>
-        <v>1159.5106249999999</v>
+        <v>579.75531249999995</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
@@ -4230,11 +4233,11 @@
         <v>127</v>
       </c>
       <c r="C86" s="6">
-        <v>18.5</v>
+        <v>9.25</v>
       </c>
       <c r="D86" s="10">
         <f>C86*1.25*1.33</f>
-        <v>30.756250000000001</v>
+        <v>15.378125000000001</v>
       </c>
       <c r="E86" s="11" t="s">
         <v>272</v>
@@ -4244,18 +4247,18 @@
       </c>
       <c r="G86" s="28">
         <f t="shared" si="54"/>
-        <v>568.99062500000002</v>
+        <v>284.49531250000001</v>
       </c>
       <c r="H86" s="28">
         <v>0</v>
       </c>
       <c r="I86" s="28">
         <f t="shared" si="55"/>
-        <v>590.52</v>
+        <v>295.26</v>
       </c>
       <c r="J86" s="28">
         <f t="shared" si="56"/>
-        <v>1159.5106249999999</v>
+        <v>579.75531249999995</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
@@ -4282,11 +4285,11 @@
         <v>129</v>
       </c>
       <c r="C88" s="6">
-        <v>20.5</v>
+        <v>10.25</v>
       </c>
       <c r="D88" s="10">
         <f>C88*1.25*1.33</f>
-        <v>34.081250000000004</v>
+        <v>17.040625000000002</v>
       </c>
       <c r="E88" s="11" t="s">
         <v>272</v>
@@ -4296,18 +4299,18 @@
       </c>
       <c r="G88" s="28">
         <f t="shared" ref="G88:G91" si="57">F88*D88</f>
-        <v>630.50312500000007</v>
+        <v>315.25156250000003</v>
       </c>
       <c r="H88" s="28">
         <v>2200</v>
       </c>
       <c r="I88" s="28">
         <f t="shared" ref="I88:I91" si="58">PRODUCT(D88,$C$2)</f>
-        <v>654.36</v>
+        <v>327.18</v>
       </c>
       <c r="J88" s="28">
         <f t="shared" ref="J88:J91" si="59">SUM(G88:I88)</f>
-        <v>3484.8631250000003</v>
+        <v>2842.4315624999999</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
@@ -4318,11 +4321,11 @@
         <v>131</v>
       </c>
       <c r="C89" s="6">
-        <v>23</v>
+        <v>11.5</v>
       </c>
       <c r="D89" s="10">
         <f>C89*1.25*1.33</f>
-        <v>38.237500000000004</v>
+        <v>19.118750000000002</v>
       </c>
       <c r="E89" s="11" t="s">
         <v>272</v>
@@ -4332,18 +4335,18 @@
       </c>
       <c r="G89" s="28">
         <f t="shared" si="57"/>
-        <v>707.39375000000007</v>
+        <v>353.69687500000003</v>
       </c>
       <c r="H89" s="28">
         <v>0</v>
       </c>
       <c r="I89" s="28">
         <f t="shared" si="58"/>
-        <v>734.16000000000008</v>
+        <v>367.08000000000004</v>
       </c>
       <c r="J89" s="28">
         <f t="shared" si="59"/>
-        <v>1441.55375</v>
+        <v>720.77687500000002</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
@@ -4354,11 +4357,11 @@
         <v>133</v>
       </c>
       <c r="C90" s="6">
-        <v>12.5</v>
+        <v>6.25</v>
       </c>
       <c r="D90" s="10">
         <f>C90*1.25*1.33</f>
-        <v>20.78125</v>
+        <v>10.390625</v>
       </c>
       <c r="E90" s="11" t="s">
         <v>272</v>
@@ -4368,18 +4371,18 @@
       </c>
       <c r="G90" s="28">
         <f t="shared" si="57"/>
-        <v>384.453125</v>
+        <v>192.2265625</v>
       </c>
       <c r="H90" s="28">
         <v>0</v>
       </c>
       <c r="I90" s="28">
         <f t="shared" si="58"/>
-        <v>399</v>
+        <v>199.5</v>
       </c>
       <c r="J90" s="28">
         <f t="shared" si="59"/>
-        <v>783.453125</v>
+        <v>391.7265625</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
@@ -4390,11 +4393,11 @@
         <v>135</v>
       </c>
       <c r="C91" s="6">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D91" s="10">
         <f>C91*1.25*1.33</f>
-        <v>19.950000000000003</v>
+        <v>9.9750000000000014</v>
       </c>
       <c r="E91" s="11" t="s">
         <v>272</v>
@@ -4404,18 +4407,18 @@
       </c>
       <c r="G91" s="28">
         <f t="shared" si="57"/>
-        <v>369.07500000000005</v>
+        <v>184.53750000000002</v>
       </c>
       <c r="H91" s="28">
         <v>0</v>
       </c>
       <c r="I91" s="28">
         <f t="shared" si="58"/>
-        <v>383.04</v>
+        <v>191.52</v>
       </c>
       <c r="J91" s="28">
         <f t="shared" si="59"/>
-        <v>752.11500000000001</v>
+        <v>376.0575</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
@@ -4442,11 +4445,11 @@
         <v>137</v>
       </c>
       <c r="C93" s="6">
-        <v>21</v>
+        <v>10.5</v>
       </c>
       <c r="D93" s="10">
         <f>C93*1.25*1.33</f>
-        <v>34.912500000000001</v>
+        <v>17.456250000000001</v>
       </c>
       <c r="E93" s="11" t="s">
         <v>272</v>
@@ -4456,18 +4459,18 @@
       </c>
       <c r="G93" s="28">
         <f t="shared" ref="G93:G95" si="60">F93*D93</f>
-        <v>645.88125000000002</v>
+        <v>322.94062500000001</v>
       </c>
       <c r="H93" s="28">
         <v>2200</v>
       </c>
       <c r="I93" s="28">
         <f t="shared" ref="I93:I95" si="61">PRODUCT(D93,$C$2)</f>
-        <v>670.32</v>
+        <v>335.16</v>
       </c>
       <c r="J93" s="28">
         <f t="shared" ref="J93:J95" si="62">SUM(G93:I93)</f>
-        <v>3516.2012500000001</v>
+        <v>2858.100625</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
@@ -4478,11 +4481,11 @@
         <v>139</v>
       </c>
       <c r="C94" s="6">
-        <v>16.5</v>
+        <v>8.25</v>
       </c>
       <c r="D94" s="10">
         <f>C94*1.25*1.33</f>
-        <v>27.431250000000002</v>
+        <v>13.715625000000001</v>
       </c>
       <c r="E94" s="11" t="s">
         <v>272</v>
@@ -4492,18 +4495,18 @@
       </c>
       <c r="G94" s="28">
         <f t="shared" si="60"/>
-        <v>507.47812500000003</v>
+        <v>253.73906250000002</v>
       </c>
       <c r="H94" s="28">
         <v>0</v>
       </c>
       <c r="I94" s="28">
         <f t="shared" si="61"/>
-        <v>526.68000000000006</v>
+        <v>263.34000000000003</v>
       </c>
       <c r="J94" s="28">
         <f t="shared" si="62"/>
-        <v>1034.1581250000002</v>
+        <v>517.07906250000008</v>
       </c>
     </row>
     <row r="95" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4514,11 +4517,11 @@
         <v>141</v>
       </c>
       <c r="C95" s="24">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D95" s="25">
         <f>C95*1.25*1.33</f>
-        <v>19.950000000000003</v>
+        <v>9.9750000000000014</v>
       </c>
       <c r="E95" s="26" t="s">
         <v>272</v>
@@ -4528,18 +4531,18 @@
       </c>
       <c r="G95" s="29">
         <f t="shared" si="60"/>
-        <v>369.07500000000005</v>
+        <v>184.53750000000002</v>
       </c>
       <c r="H95" s="29">
         <v>0</v>
       </c>
       <c r="I95" s="29">
         <f t="shared" si="61"/>
-        <v>383.04</v>
+        <v>191.52</v>
       </c>
       <c r="J95" s="29">
         <f t="shared" si="62"/>
-        <v>752.11500000000001</v>
+        <v>376.0575</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
@@ -6795,17 +6798,17 @@
       </c>
     </row>
     <row r="168" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A168" s="33" t="s">
+      <c r="A168" s="34" t="s">
         <v>274</v>
       </c>
-      <c r="B168" s="34"/>
-      <c r="C168" s="32">
+      <c r="B168" s="35"/>
+      <c r="C168" s="33">
         <f>SUM(C6:C167)</f>
-        <v>1782</v>
-      </c>
-      <c r="D168" s="32">
+        <v>1604</v>
+      </c>
+      <c r="D168" s="33">
         <f>SUM(D6:D167)</f>
-        <v>2962.5750000000003</v>
+        <v>2666.6500000000005</v>
       </c>
       <c r="E168" s="27"/>
       <c r="F168" s="32">
@@ -6814,7 +6817,7 @@
       </c>
       <c r="G168" s="32">
         <f>SUM(G6:G167)</f>
-        <v>56112.442312499996</v>
+        <v>50637.8298125</v>
       </c>
       <c r="H168" s="32">
         <f>SUM(H6:H167)</f>
@@ -6822,16 +6825,16 @@
       </c>
       <c r="I168" s="32">
         <f>SUM(I6:I167)</f>
-        <v>56881.440000000024</v>
+        <v>51199.680000000008</v>
       </c>
       <c r="J168" s="32">
         <f>SUM(J6:J167)</f>
-        <v>163793.88231250001</v>
+        <v>152637.50981249998</v>
       </c>
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A170" s="35"/>
-      <c r="B170" s="36"/>
+      <c r="A170" s="36"/>
+      <c r="B170" s="37"/>
       <c r="E170" s="14"/>
       <c r="F170" s="14"/>
       <c r="G170" s="14"/>

</xml_diff>

<commit_message>
docs: add project network diagram
</commit_message>
<xml_diff>
--- a/docs/resources/tables/cost-analysis-2023-02-03.xlsx
+++ b/docs/resources/tables/cost-analysis-2023-02-03.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jahrim\Desktop\Projects\pm-project\docs\resources\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E774235-D9B2-4B8C-80D8-0219AF4A4D66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E64D2079-F2F5-4DF2-BA55-85B16449BAD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Task Analysis" sheetId="1" r:id="rId1"/>
@@ -520,15 +520,9 @@
     <t>Handle User Permissions</t>
   </si>
   <si>
-    <t>A4.1</t>
-  </si>
-  <si>
     <t>Get User Profile Information</t>
   </si>
   <si>
-    <t>A4.2</t>
-  </si>
-  <si>
     <t>Update User Profile Information</t>
   </si>
   <si>
@@ -926,6 +920,12 @@
   </si>
   <si>
     <t>Costi di Manodopera</t>
+  </si>
+  <si>
+    <t>A3.1</t>
+  </si>
+  <si>
+    <t>A3.2</t>
   </si>
 </sst>
 </file>
@@ -1595,8 +1595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A147" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C177" sqref="C177"/>
+    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1613,7 +1613,7 @@
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="38" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B2" s="39"/>
       <c r="C2" s="30">
@@ -1629,36 +1629,36 @@
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>293</v>
-      </c>
-      <c r="H4" s="4" t="s">
+      <c r="J4" s="5" t="s">
         <v>277</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="2"/>
@@ -1684,7 +1684,7 @@
         <v>14.9625</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F6" s="28">
         <v>17.399999999999999</v>
@@ -1720,7 +1720,7 @@
         <v>15.793750000000001</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F7" s="28">
         <v>18</v>
@@ -1756,7 +1756,7 @@
         <v>11.637500000000001</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F8" s="28">
         <v>18</v>
@@ -1792,7 +1792,7 @@
         <v>2.078125</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F9" s="28">
         <v>18</v>
@@ -1828,7 +1828,7 @@
         <v>2.078125</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F10" s="28">
         <v>18</v>
@@ -1864,7 +1864,7 @@
         <v>2.4937500000000004</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F11" s="28">
         <v>18</v>
@@ -1900,7 +1900,7 @@
         <v>2.078125</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F12" s="28">
         <v>18</v>
@@ -1936,7 +1936,7 @@
         <v>2.078125</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F13" s="28">
         <v>18</v>
@@ -1972,7 +1972,7 @@
         <v>2.078125</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F14" s="28">
         <v>18</v>
@@ -2024,7 +2024,7 @@
         <v>11.637500000000001</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F16" s="28">
         <v>17.399999999999999</v>
@@ -2060,7 +2060,7 @@
         <v>14.9625</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F17" s="28">
         <v>18</v>
@@ -2096,7 +2096,7 @@
         <v>14.9625</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F18" s="28">
         <v>18</v>
@@ -2132,7 +2132,7 @@
         <v>3.3250000000000002</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F19" s="28">
         <v>18</v>
@@ -2168,7 +2168,7 @@
         <v>3.3250000000000002</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F20" s="28">
         <v>18</v>
@@ -2220,7 +2220,7 @@
         <v>15.793750000000001</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F22" s="28">
         <v>17.399999999999999</v>
@@ -2256,7 +2256,7 @@
         <v>24.106250000000003</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F23" s="28">
         <v>18</v>
@@ -2292,7 +2292,7 @@
         <v>9.9750000000000014</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F24" s="28">
         <v>18</v>
@@ -2328,7 +2328,7 @@
         <v>6.65</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F25" s="28">
         <v>18</v>
@@ -2351,7 +2351,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>85</v>
@@ -2364,7 +2364,7 @@
         <v>6.65</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F26" s="28">
         <v>18</v>
@@ -2412,7 +2412,7 @@
         <v>16.625</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F28" s="28">
         <v>17.399999999999999</v>
@@ -2448,7 +2448,7 @@
         <v>14.9625</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F29" s="28">
         <v>18</v>
@@ -2484,7 +2484,7 @@
         <v>12.46875</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F30" s="28">
         <v>18</v>
@@ -2536,7 +2536,7 @@
         <v>14.131250000000001</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F32" s="28">
         <v>17.399999999999999</v>
@@ -2572,7 +2572,7 @@
         <v>13.3</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F33" s="28">
         <v>18</v>
@@ -2608,7 +2608,7 @@
         <v>16.625</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F34" s="28">
         <v>18</v>
@@ -2660,7 +2660,7 @@
         <v>26.6</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F36" s="28">
         <v>17.399999999999999</v>
@@ -2696,7 +2696,7 @@
         <v>29.925000000000001</v>
       </c>
       <c r="E37" s="11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F37" s="28">
         <v>18</v>
@@ -2732,7 +2732,7 @@
         <v>13.3</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F38" s="28">
         <v>18</v>
@@ -2784,7 +2784,7 @@
         <v>14.9625</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F40" s="28">
         <v>17.399999999999999</v>
@@ -2820,7 +2820,7 @@
         <v>16.625</v>
       </c>
       <c r="E41" s="11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F41" s="28">
         <v>18</v>
@@ -2856,7 +2856,7 @@
         <v>7.4812500000000002</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F42" s="28">
         <v>18</v>
@@ -2908,7 +2908,7 @@
         <v>9.9750000000000014</v>
       </c>
       <c r="E44" s="11" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F44" s="28">
         <v>17.399999999999999</v>
@@ -2944,7 +2944,7 @@
         <v>12.46875</v>
       </c>
       <c r="E45" s="11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F45" s="28">
         <v>18</v>
@@ -2980,7 +2980,7 @@
         <v>11.637500000000001</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F46" s="28">
         <v>18</v>
@@ -3032,7 +3032,7 @@
         <v>14.9625</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F48" s="28">
         <v>17.399999999999999</v>
@@ -3068,7 +3068,7 @@
         <v>27.431250000000002</v>
       </c>
       <c r="E49" s="11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F49" s="28">
         <v>18</v>
@@ -3104,7 +3104,7 @@
         <v>17.456250000000001</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F50" s="28">
         <v>18</v>
@@ -3156,7 +3156,7 @@
         <v>17.456250000000001</v>
       </c>
       <c r="E52" s="11" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F52" s="28">
         <v>17.399999999999999</v>
@@ -3192,7 +3192,7 @@
         <v>33.25</v>
       </c>
       <c r="E53" s="11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F53" s="28">
         <v>18</v>
@@ -3228,7 +3228,7 @@
         <v>22.443750000000001</v>
       </c>
       <c r="E54" s="11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F54" s="28">
         <v>18</v>
@@ -3251,7 +3251,7 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B55" s="8" t="s">
         <v>86</v>
@@ -3264,7 +3264,7 @@
         <v>7.4812500000000002</v>
       </c>
       <c r="E55" s="11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F55" s="28">
         <v>18</v>
@@ -3316,7 +3316,7 @@
         <v>25.768750000000001</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F57" s="28">
         <v>17.399999999999999</v>
@@ -3352,7 +3352,7 @@
         <v>39.900000000000006</v>
       </c>
       <c r="E58" s="11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F58" s="28">
         <v>18</v>
@@ -3388,7 +3388,7 @@
         <v>14.9625</v>
       </c>
       <c r="E59" s="11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F59" s="28">
         <v>18</v>
@@ -3440,7 +3440,7 @@
         <v>28.262500000000003</v>
       </c>
       <c r="E61" s="11" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F61" s="28">
         <v>17.399999999999999</v>
@@ -3476,7 +3476,7 @@
         <v>25.768750000000001</v>
       </c>
       <c r="E62" s="11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F62" s="28">
         <v>18</v>
@@ -3512,7 +3512,7 @@
         <v>20.78125</v>
       </c>
       <c r="E63" s="11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F63" s="28">
         <v>18</v>
@@ -3564,7 +3564,7 @@
         <v>24.9375</v>
       </c>
       <c r="E65" s="11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F65" s="28">
         <v>17.399999999999999</v>
@@ -3600,7 +3600,7 @@
         <v>4.15625</v>
       </c>
       <c r="E66" s="11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F66" s="28">
         <v>18</v>
@@ -3636,7 +3636,7 @@
         <v>12.46875</v>
       </c>
       <c r="E67" s="11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F67" s="28">
         <v>18</v>
@@ -3659,7 +3659,7 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B68" s="8" t="s">
         <v>102</v>
@@ -3672,7 +3672,7 @@
         <v>9.9750000000000014</v>
       </c>
       <c r="E68" s="11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F68" s="28">
         <v>18</v>
@@ -3695,7 +3695,7 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B69" s="8" t="s">
         <v>103</v>
@@ -3708,7 +3708,7 @@
         <v>120.53125</v>
       </c>
       <c r="E69" s="8" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="F69" s="28">
         <v>17.2</v>
@@ -3731,10 +3731,10 @@
     </row>
     <row r="70" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="23" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B70" s="23" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C70" s="24">
         <v>21.25</v>
@@ -3744,7 +3744,7 @@
         <v>35.328125</v>
       </c>
       <c r="E70" s="26" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F70" s="29">
         <v>18</v>
@@ -3767,10 +3767,10 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C71" s="12"/>
       <c r="D71" s="2"/>
@@ -3796,7 +3796,7 @@
         <v>17.871874999999999</v>
       </c>
       <c r="E72" s="11" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F72" s="28">
         <v>18.5</v>
@@ -3832,7 +3832,7 @@
         <v>15.378125000000001</v>
       </c>
       <c r="E73" s="11" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F73" s="28">
         <v>18.5</v>
@@ -3868,7 +3868,7 @@
         <v>17.040625000000002</v>
       </c>
       <c r="E74" s="11" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F74" s="28">
         <v>18.5</v>
@@ -3920,7 +3920,7 @@
         <v>17.871874999999999</v>
       </c>
       <c r="E76" s="11" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F76" s="28">
         <v>18.5</v>
@@ -3956,7 +3956,7 @@
         <v>17.040625000000002</v>
       </c>
       <c r="E77" s="11" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F77" s="28">
         <v>18.5</v>
@@ -3992,7 +3992,7 @@
         <v>18.287500000000001</v>
       </c>
       <c r="E78" s="11" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F78" s="28">
         <v>18.5</v>
@@ -4044,7 +4044,7 @@
         <v>17.871874999999999</v>
       </c>
       <c r="E80" s="11" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F80" s="28">
         <v>18.5</v>
@@ -4080,7 +4080,7 @@
         <v>15.378125000000001</v>
       </c>
       <c r="E81" s="11" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F81" s="28">
         <v>18.5</v>
@@ -4116,7 +4116,7 @@
         <v>12.884375</v>
       </c>
       <c r="E82" s="11" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F82" s="28">
         <v>18.5</v>
@@ -4168,7 +4168,7 @@
         <v>17.871874999999999</v>
       </c>
       <c r="E84" s="11" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F84" s="28">
         <v>18.5</v>
@@ -4204,7 +4204,7 @@
         <v>15.378125000000001</v>
       </c>
       <c r="E85" s="11" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F85" s="28">
         <v>18.5</v>
@@ -4240,7 +4240,7 @@
         <v>15.378125000000001</v>
       </c>
       <c r="E86" s="11" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F86" s="28">
         <v>18.5</v>
@@ -4292,7 +4292,7 @@
         <v>17.040625000000002</v>
       </c>
       <c r="E88" s="11" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F88" s="28">
         <v>18.5</v>
@@ -4328,7 +4328,7 @@
         <v>19.118750000000002</v>
       </c>
       <c r="E89" s="11" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F89" s="28">
         <v>18.5</v>
@@ -4364,7 +4364,7 @@
         <v>10.390625</v>
       </c>
       <c r="E90" s="11" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F90" s="28">
         <v>18.5</v>
@@ -4400,7 +4400,7 @@
         <v>9.9750000000000014</v>
       </c>
       <c r="E91" s="11" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F91" s="28">
         <v>18.5</v>
@@ -4452,7 +4452,7 @@
         <v>17.456250000000001</v>
       </c>
       <c r="E93" s="11" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F93" s="28">
         <v>18.5</v>
@@ -4488,7 +4488,7 @@
         <v>13.715625000000001</v>
       </c>
       <c r="E94" s="11" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F94" s="28">
         <v>18.5</v>
@@ -4524,7 +4524,7 @@
         <v>9.9750000000000014</v>
       </c>
       <c r="E95" s="26" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F95" s="29">
         <v>18.5</v>
@@ -4547,10 +4547,10 @@
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C96" s="12"/>
       <c r="D96" s="2"/>
@@ -4576,7 +4576,7 @@
         <v>19.118750000000002</v>
       </c>
       <c r="E97" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F97" s="28">
         <v>19.600000000000001</v>
@@ -4612,7 +4612,7 @@
         <v>16.625</v>
       </c>
       <c r="E98" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F98" s="28">
         <v>19.600000000000001</v>
@@ -4648,7 +4648,7 @@
         <v>7.4812500000000002</v>
       </c>
       <c r="E99" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F99" s="28">
         <v>19.600000000000001</v>
@@ -4684,7 +4684,7 @@
         <v>13.3</v>
       </c>
       <c r="E100" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F100" s="28">
         <v>19.600000000000001</v>
@@ -4736,7 +4736,7 @@
         <v>16.625</v>
       </c>
       <c r="E102" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F102" s="28">
         <v>19.600000000000001</v>
@@ -4772,7 +4772,7 @@
         <v>4.9875000000000007</v>
       </c>
       <c r="E103" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F103" s="28">
         <v>19.600000000000001</v>
@@ -4808,7 +4808,7 @@
         <v>7.4812500000000002</v>
       </c>
       <c r="E104" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F104" s="28">
         <v>19.600000000000001</v>
@@ -4844,7 +4844,7 @@
         <v>29.925000000000001</v>
       </c>
       <c r="E105" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F105" s="28">
         <v>19.600000000000001</v>
@@ -4883,10 +4883,10 @@
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="B107" s="8" t="s">
         <v>158</v>
-      </c>
-      <c r="B107" s="8" t="s">
-        <v>159</v>
       </c>
       <c r="C107" s="6">
         <v>14</v>
@@ -4896,7 +4896,7 @@
         <v>23.275000000000002</v>
       </c>
       <c r="E107" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F107" s="28">
         <v>19.600000000000001</v>
@@ -4919,10 +4919,10 @@
     </row>
     <row r="108" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="22" t="s">
-        <v>160</v>
+        <v>293</v>
       </c>
       <c r="B108" s="23" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C108" s="24">
         <v>6.5</v>
@@ -4932,7 +4932,7 @@
         <v>10.80625</v>
       </c>
       <c r="E108" s="26" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F108" s="29">
         <v>19.600000000000001</v>
@@ -4955,10 +4955,10 @@
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C109" s="12"/>
       <c r="D109" s="2"/>
@@ -4971,10 +4971,10 @@
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B110" s="8" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C110" s="6">
         <v>7</v>
@@ -4984,7 +4984,7 @@
         <v>11.637500000000001</v>
       </c>
       <c r="E110" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F110" s="28">
         <v>19.600000000000001</v>
@@ -5007,10 +5007,10 @@
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="9" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C111" s="6">
         <v>4.5</v>
@@ -5020,7 +5020,7 @@
         <v>7.4812500000000002</v>
       </c>
       <c r="E111" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F111" s="28">
         <v>19.600000000000001</v>
@@ -5043,10 +5043,10 @@
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="9" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B112" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C112" s="6">
         <v>7.5</v>
@@ -5056,7 +5056,7 @@
         <v>12.46875</v>
       </c>
       <c r="E112" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F112" s="28">
         <v>19.600000000000001</v>
@@ -5095,10 +5095,10 @@
     </row>
     <row r="114" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="22" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B114" s="23" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C114" s="24">
         <v>6</v>
@@ -5108,7 +5108,7 @@
         <v>9.9750000000000014</v>
       </c>
       <c r="E114" s="26" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F114" s="29">
         <v>19.600000000000001</v>
@@ -5131,10 +5131,10 @@
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C115" s="12"/>
       <c r="D115" s="2"/>
@@ -5147,10 +5147,10 @@
     </row>
     <row r="116" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="22" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B116" s="23" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C116" s="24">
         <v>15</v>
@@ -5160,7 +5160,7 @@
         <v>24.9375</v>
       </c>
       <c r="E116" s="26" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F116" s="29">
         <v>19.600000000000001</v>
@@ -5183,10 +5183,10 @@
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C117" s="12"/>
       <c r="D117" s="2"/>
@@ -5199,10 +5199,10 @@
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="9" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B118" s="8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C118" s="6">
         <v>21.5</v>
@@ -5212,7 +5212,7 @@
         <v>35.743749999999999</v>
       </c>
       <c r="E118" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F118" s="28">
         <v>19.600000000000001</v>
@@ -5235,10 +5235,10 @@
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="9" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B119" s="8" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C119" s="6">
         <v>3</v>
@@ -5248,7 +5248,7 @@
         <v>4.9875000000000007</v>
       </c>
       <c r="E119" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F119" s="28">
         <v>19.600000000000001</v>
@@ -5271,10 +5271,10 @@
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="9" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B120" s="8" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C120" s="6">
         <v>3</v>
@@ -5284,7 +5284,7 @@
         <v>4.9875000000000007</v>
       </c>
       <c r="E120" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F120" s="28">
         <v>19.600000000000001</v>
@@ -5307,10 +5307,10 @@
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="9" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B121" s="8" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C121" s="6">
         <v>8.5</v>
@@ -5320,7 +5320,7 @@
         <v>14.131250000000001</v>
       </c>
       <c r="E121" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F121" s="28">
         <v>19.600000000000001</v>
@@ -5343,10 +5343,10 @@
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B122" s="8" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C122" s="6">
         <v>3</v>
@@ -5356,7 +5356,7 @@
         <v>4.9875000000000007</v>
       </c>
       <c r="E122" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F122" s="28">
         <v>19.600000000000001</v>
@@ -5379,10 +5379,10 @@
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="9" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B123" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C123" s="6">
         <v>3</v>
@@ -5392,7 +5392,7 @@
         <v>4.9875000000000007</v>
       </c>
       <c r="E123" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F123" s="28">
         <v>19.600000000000001</v>
@@ -5415,10 +5415,10 @@
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="9" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B124" s="8" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C124" s="6">
         <v>3</v>
@@ -5428,7 +5428,7 @@
         <v>4.9875000000000007</v>
       </c>
       <c r="E124" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F124" s="28">
         <v>19.600000000000001</v>
@@ -5451,10 +5451,10 @@
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="9" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B125" s="8" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C125" s="6">
         <v>9.5</v>
@@ -5464,7 +5464,7 @@
         <v>15.793750000000001</v>
       </c>
       <c r="E125" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F125" s="28">
         <v>19.600000000000001</v>
@@ -5487,10 +5487,10 @@
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="9" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B126" s="8" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C126" s="6">
         <v>8.5</v>
@@ -5500,7 +5500,7 @@
         <v>14.131250000000001</v>
       </c>
       <c r="E126" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F126" s="28">
         <v>19.600000000000001</v>
@@ -5539,10 +5539,10 @@
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="9" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B128" s="8" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C128" s="6">
         <v>19.5</v>
@@ -5552,7 +5552,7 @@
         <v>32.418750000000003</v>
       </c>
       <c r="E128" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F128" s="28">
         <v>19.600000000000001</v>
@@ -5575,10 +5575,10 @@
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="9" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B129" s="8" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C129" s="6">
         <v>22.5</v>
@@ -5588,7 +5588,7 @@
         <v>37.40625</v>
       </c>
       <c r="E129" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F129" s="28">
         <v>19.600000000000001</v>
@@ -5611,10 +5611,10 @@
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="9" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B130" s="8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C130" s="6">
         <v>26</v>
@@ -5624,7 +5624,7 @@
         <v>43.225000000000001</v>
       </c>
       <c r="E130" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F130" s="28">
         <v>19.600000000000001</v>
@@ -5663,10 +5663,10 @@
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B132" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C132" s="6">
         <v>18</v>
@@ -5676,7 +5676,7 @@
         <v>29.925000000000001</v>
       </c>
       <c r="E132" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F132" s="28">
         <v>19.600000000000001</v>
@@ -5715,10 +5715,10 @@
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" s="9" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B134" s="8" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C134" s="6">
         <v>84</v>
@@ -5728,7 +5728,7 @@
         <v>139.65</v>
       </c>
       <c r="E134" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F134" s="28">
         <v>19.600000000000001</v>
@@ -5751,10 +5751,10 @@
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="9" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B135" s="8" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C135" s="6">
         <v>74</v>
@@ -5764,7 +5764,7 @@
         <v>123.02500000000001</v>
       </c>
       <c r="E135" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F135" s="28">
         <v>19.600000000000001</v>
@@ -5803,10 +5803,10 @@
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" s="9" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B137" s="8" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C137" s="6">
         <v>10.5</v>
@@ -5816,7 +5816,7 @@
         <v>17.456250000000001</v>
       </c>
       <c r="E137" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F137" s="28">
         <v>19.600000000000001</v>
@@ -5839,10 +5839,10 @@
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" s="9" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B138" s="8" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C138" s="6">
         <v>15.5</v>
@@ -5852,7 +5852,7 @@
         <v>25.768750000000001</v>
       </c>
       <c r="E138" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F138" s="28">
         <v>19.600000000000001</v>
@@ -5875,10 +5875,10 @@
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="9" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B139" s="8" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C139" s="6">
         <v>12</v>
@@ -5888,7 +5888,7 @@
         <v>19.950000000000003</v>
       </c>
       <c r="E139" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F139" s="28">
         <v>19.600000000000001</v>
@@ -5911,10 +5911,10 @@
     </row>
     <row r="140" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A140" s="22" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B140" s="23" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C140" s="24">
         <v>11</v>
@@ -5924,7 +5924,7 @@
         <v>18.287500000000001</v>
       </c>
       <c r="E140" s="26" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F140" s="29">
         <v>19.600000000000001</v>
@@ -5947,10 +5947,10 @@
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C141" s="12"/>
       <c r="D141" s="2"/>
@@ -5963,10 +5963,10 @@
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="9" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B142" s="8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C142" s="6">
         <v>19</v>
@@ -5976,7 +5976,7 @@
         <v>31.587500000000002</v>
       </c>
       <c r="E142" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F142" s="28">
         <v>19.600000000000001</v>
@@ -5999,10 +5999,10 @@
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="9" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B143" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C143" s="6">
         <v>11</v>
@@ -6012,7 +6012,7 @@
         <v>18.287500000000001</v>
       </c>
       <c r="E143" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F143" s="28">
         <v>19.600000000000001</v>
@@ -6051,10 +6051,10 @@
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" s="9" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B145" s="8" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C145" s="6">
         <v>18</v>
@@ -6064,7 +6064,7 @@
         <v>29.925000000000001</v>
       </c>
       <c r="E145" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F145" s="28">
         <v>19.600000000000001</v>
@@ -6087,10 +6087,10 @@
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" s="9" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B146" s="8" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C146" s="6">
         <v>12</v>
@@ -6100,7 +6100,7 @@
         <v>19.950000000000003</v>
       </c>
       <c r="E146" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F146" s="28">
         <v>19.600000000000001</v>
@@ -6123,10 +6123,10 @@
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" s="9" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B147" s="8" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C147" s="6">
         <v>9</v>
@@ -6136,7 +6136,7 @@
         <v>14.9625</v>
       </c>
       <c r="E147" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F147" s="28">
         <v>19.600000000000001</v>
@@ -6175,10 +6175,10 @@
     </row>
     <row r="149" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="22" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B149" s="23" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C149" s="24">
         <v>19</v>
@@ -6188,7 +6188,7 @@
         <v>31.587500000000002</v>
       </c>
       <c r="E149" s="26" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F149" s="29">
         <v>19.600000000000001</v>
@@ -6211,10 +6211,10 @@
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C150" s="12"/>
       <c r="D150" s="2"/>
@@ -6227,10 +6227,10 @@
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" s="9" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B151" s="8" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C151" s="6">
         <v>5.5</v>
@@ -6240,7 +6240,7 @@
         <v>9.1437500000000007</v>
       </c>
       <c r="E151" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F151" s="28">
         <v>19.600000000000001</v>
@@ -6263,10 +6263,10 @@
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="9" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B152" s="8" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C152" s="6">
         <v>4.5</v>
@@ -6276,7 +6276,7 @@
         <v>7.4812500000000002</v>
       </c>
       <c r="E152" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F152" s="28">
         <v>19.600000000000001</v>
@@ -6299,10 +6299,10 @@
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" s="9" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B153" s="8" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C153" s="6">
         <v>17</v>
@@ -6312,7 +6312,7 @@
         <v>28.262500000000003</v>
       </c>
       <c r="E153" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F153" s="28">
         <v>19.600000000000001</v>
@@ -6335,10 +6335,10 @@
     </row>
     <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" s="9" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B154" s="8" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C154" s="6">
         <v>8.5</v>
@@ -6348,7 +6348,7 @@
         <v>14.131250000000001</v>
       </c>
       <c r="E154" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F154" s="28">
         <v>19.600000000000001</v>
@@ -6371,10 +6371,10 @@
     </row>
     <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" s="9" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B155" s="8" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C155" s="6">
         <v>5</v>
@@ -6384,7 +6384,7 @@
         <v>8.3125</v>
       </c>
       <c r="E155" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F155" s="28">
         <v>19.600000000000001</v>
@@ -6407,10 +6407,10 @@
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" s="9" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B156" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C156" s="6">
         <v>7</v>
@@ -6420,7 +6420,7 @@
         <v>11.637500000000001</v>
       </c>
       <c r="E156" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F156" s="28">
         <v>19.600000000000001</v>
@@ -6443,10 +6443,10 @@
     </row>
     <row r="157" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A157" s="22" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B157" s="23" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C157" s="24">
         <v>8.5</v>
@@ -6456,7 +6456,7 @@
         <v>14.131250000000001</v>
       </c>
       <c r="E157" s="26" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F157" s="29">
         <v>19.600000000000001</v>
@@ -6479,10 +6479,10 @@
     </row>
     <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C158" s="12"/>
       <c r="D158" s="2"/>
@@ -6495,10 +6495,10 @@
     </row>
     <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" s="9" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B159" s="8" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C159" s="6">
         <v>7.5</v>
@@ -6508,7 +6508,7 @@
         <v>12.46875</v>
       </c>
       <c r="E159" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F159" s="28">
         <v>19.600000000000001</v>
@@ -6531,10 +6531,10 @@
     </row>
     <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" s="9" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B160" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C160" s="6">
         <v>13</v>
@@ -6544,7 +6544,7 @@
         <v>21.612500000000001</v>
       </c>
       <c r="E160" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F160" s="28">
         <v>19.600000000000001</v>
@@ -6567,10 +6567,10 @@
     </row>
     <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" s="9" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B161" s="8" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C161" s="6">
         <v>10.5</v>
@@ -6580,7 +6580,7 @@
         <v>17.456250000000001</v>
       </c>
       <c r="E161" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F161" s="28">
         <v>19.600000000000001</v>
@@ -6603,10 +6603,10 @@
     </row>
     <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" s="9" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B162" s="8" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C162" s="6">
         <v>11</v>
@@ -6616,7 +6616,7 @@
         <v>18.287500000000001</v>
       </c>
       <c r="E162" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F162" s="28">
         <v>19.600000000000001</v>
@@ -6639,10 +6639,10 @@
     </row>
     <row r="163" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A163" s="22" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B163" s="23" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C163" s="24">
         <v>9</v>
@@ -6652,7 +6652,7 @@
         <v>14.9625</v>
       </c>
       <c r="E163" s="23" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F163" s="29">
         <v>19.600000000000001</v>
@@ -6675,10 +6675,10 @@
     </row>
     <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C164" s="12"/>
       <c r="D164" s="2"/>
@@ -6691,10 +6691,10 @@
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" s="9" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B165" s="8" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C165" s="6">
         <v>107.5</v>
@@ -6704,7 +6704,7 @@
         <v>178.71875</v>
       </c>
       <c r="E165" s="11" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="F165" s="28">
         <v>21.79</v>
@@ -6727,10 +6727,10 @@
     </row>
     <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B166" s="8" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C166" s="6">
         <v>57.5</v>
@@ -6740,7 +6740,7 @@
         <v>95.59375</v>
       </c>
       <c r="E166" s="11" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F166" s="28">
         <v>18</v>
@@ -6763,10 +6763,10 @@
     </row>
     <row r="167" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B167" s="8" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C167" s="6">
         <v>38</v>
@@ -6776,7 +6776,7 @@
         <v>63.175000000000004</v>
       </c>
       <c r="E167" s="11" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="F167" s="28">
         <v>21.79</v>
@@ -6799,7 +6799,7 @@
     </row>
     <row r="168" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="34" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B168" s="35"/>
       <c r="C168" s="33">

</xml_diff>